<commit_message>
Better derived importance chart
</commit_message>
<xml_diff>
--- a/TotalDominance.xlsx
+++ b/TotalDominance.xlsx
@@ -11,11 +11,12 @@
     <sheet name="DS_Train" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="DS_Car" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Combined_Data" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Pivot Table_Combined_Data_1" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Pivot Table_Combined_Data_2" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Pivot Table_Combined_Data_1" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="25">
   <si>
     <t xml:space="preserve">Mode</t>
   </si>
@@ -99,6 +100,9 @@
   <si>
     <t xml:space="preserve">Data</t>
   </si>
+  <si>
+    <t xml:space="preserve">Total Result</t>
+  </si>
 </sst>
 </file>
 
@@ -107,11 +111,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -133,14 +138,20 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <sz val="20"/>
+      <sz val="16"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -153,7 +164,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="29">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -177,13 +188,6 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
       <right style="medium"/>
       <top style="medium"/>
       <bottom style="thin"/>
@@ -198,13 +202,6 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
-      <right/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
       <right/>
       <top/>
       <bottom style="thin"/>
@@ -233,15 +230,29 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
       <right/>
-      <top style="thin"/>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="medium"/>
-      <top style="thin"/>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -261,15 +272,99 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right/>
+      <right style="medium"/>
       <top/>
       <bottom style="medium"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
+      <right/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
       <right style="medium"/>
       <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
       <bottom style="medium"/>
       <diagonal/>
     </border>
@@ -298,18 +393,26 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -318,7 +421,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -326,59 +429,119 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="24" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="24" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="25" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="26" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="27" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="28" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -390,12 +553,12 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Pivot Table Corner" xfId="20"/>
-    <cellStyle name="Pivot Table Value" xfId="21"/>
+    <cellStyle name="Pivot Table Category" xfId="20"/>
+    <cellStyle name="Pivot Table Corner" xfId="21"/>
     <cellStyle name="Pivot Table Field" xfId="22"/>
-    <cellStyle name="Pivot Table Category" xfId="23"/>
+    <cellStyle name="Pivot Table Result" xfId="23"/>
     <cellStyle name="Pivot Table Title" xfId="24"/>
-    <cellStyle name="Pivot Table Result" xfId="25"/>
+    <cellStyle name="Pivot Table Value" xfId="25"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -407,7 +570,7 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF7E0021"/>
+      <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
@@ -435,32 +598,32 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF83CAFF"/>
+      <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FFAECF00"/>
-      <rgbColor rgb="FFFFD320"/>
-      <rgbColor rgb="FFFF950E"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF004586"/>
-      <rgbColor rgb="FF579D1C"/>
+      <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF314004"/>
+      <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF4B1F6F"/>
+      <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -472,15 +635,15 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="2000" spc="-1" strike="noStrike">
+              <a:defRPr b="0" sz="1600" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" sz="2000" spc="-1" strike="noStrike">
+              <a:rPr b="0" sz="1600" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Percent Relative Importance Trains vs. Cars</a:t>
+              <a:t>Derived Importance Trains vs. Cars</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -495,20 +658,9 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.0677744541536142"/>
-          <c:y val="0.0822875665663348"/>
-          <c:w val="0.901877193395671"/>
-          <c:h val="0.728501968048159"/>
-        </c:manualLayout>
-      </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
-        <c:grouping val="percentStacked"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -519,7 +671,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Can interact with others</c:v>
+                  <c:v>Car</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -540,9 +692,6 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="ffffff"/>
-                    </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
@@ -552,7 +701,7 @@
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
+            <c:showPercent val="0"/>
             <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
@@ -560,12 +709,36 @@
             <c:strRef>
               <c:f>pt@categories</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Car</c:v>
+                  <c:v>Can interact with others</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Train</c:v>
+                  <c:v>Gives me the ability to work read and sleep</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Has comfortable seating</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Is a good value for the money</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Is clean</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Is convenient to use</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Is good for the environment</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Is mostly on time</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Is relaxing</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Is safe from accidents</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -575,12 +748,36 @@
               <c:f>pt@data 0</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.00328508839711066</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.7631838125845</c:v>
+                  <c:v>5.92157252328551</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0228178449402206</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.9687740199064</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.2528246248874</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.70519652984693</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26.2281191240734</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19.2840674894714</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.67337159052342</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.939971164668175</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -595,7 +792,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Gives me the ability to work read and sleep</c:v>
+                  <c:v>Train</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -625,7 +822,7 @@
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
+            <c:showPercent val="0"/>
             <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
@@ -633,12 +830,36 @@
             <c:strRef>
               <c:f>pt@categories</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Car</c:v>
+                  <c:v>Can interact with others</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Train</c:v>
+                  <c:v>Gives me the ability to work read and sleep</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Has comfortable seating</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Is a good value for the money</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Is clean</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Is convenient to use</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Is good for the environment</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Is mostly on time</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Is relaxing</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Is safe from accidents</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -648,604 +869,35 @@
               <c:f>pt@data 1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>5.92157252328551</c:v>
+                  <c:v>12.7631838125845</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6.64197827475527</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>pt@label 2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Has comfortable seating</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ffd320"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>pt@categories</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Car</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Train</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>pt@data 2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.0228178449402206</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>17.5463780763681</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>pt@label 3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Is a good value for the money</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="579d1c"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>pt@categories</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Car</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Train</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>pt@data 3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>11.9687740199064</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>1.4533175326318</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>pt@label 4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Is clean</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="7e0021"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="ffffff"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>pt@categories</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Car</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Train</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>pt@data 4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>29.2528246248874</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>1.31833454233002</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>pt@label 5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Is convenient to use</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="83caff"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>pt@categories</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Car</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Train</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>pt@data 5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>3.70519652984693</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>0.758193902581064</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>pt@label 6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Is good for the environment</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="314004"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="ffffff"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>pt@categories</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Car</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Train</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>pt@data 6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>26.2281191240734</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
                   <c:v>28.4042171216637</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>pt@label 7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Is mostly on time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="aecf00"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>pt@categories</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Car</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Train</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>pt@data 7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>19.2840674894714</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="7">
                   <c:v>16.7897813147668</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="8"/>
-          <c:order val="8"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>pt@label 8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Is relaxing</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4b1f6f"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="ffffff"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>pt@categories</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Car</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Train</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>pt@data 8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>2.67337159052342</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="8">
                   <c:v>11.6132366222505</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="9"/>
-          <c:order val="9"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>pt@label 9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Is safe from accidents</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ff950e"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>pt@categories</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Car</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Train</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>pt@data 9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.939971164668175</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>2.7113788000683</c:v>
                 </c:pt>
               </c:numCache>
@@ -1253,21 +905,66 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:overlap val="100"/>
-        <c:axId val="69853720"/>
-        <c:axId val="13785799"/>
+        <c:overlap val="0"/>
+        <c:axId val="73800026"/>
+        <c:axId val="79094054"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="69853720"/>
+        <c:axId val="73800026"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="79094054"/>
+        <c:crossesAt val="0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="79094054"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000"/>
+              <a:bodyPr rot="0"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -1279,19 +976,11 @@
                   <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>Mode of Transport</a:t>
+                  <a:t>Percentage Relative Importance</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.0071600169579349"/>
-              <c:y val="0.360437117984812"/>
-            </c:manualLayout>
-          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1322,53 +1011,8 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13785799"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="13785799"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="[$-409]0%" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="69853720"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="73800026"/>
+        <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -1381,17 +1025,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.156841039169042"/>
-          <c:y val="0.86482982171799"/>
-          <c:w val="0.724568386838448"/>
-          <c:h val="0.13484602917342"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1429,16 +1063,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>39960</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>694080</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>9720</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>476280</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>137880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1446,8 +1080,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="852480" y="38160"/>
-        <a:ext cx="15284520" cy="7774200"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="16732080" cy="9241200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1797,7 +1431,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="0" outlineData="0" compact="0" compactData="0">
-  <location ref="A1:K4" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <location ref="A1:L5" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0" outline="0">
       <items count="2">
@@ -1838,6 +1472,49 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="0" outlineData="0" compact="0" compactData="0">
+  <location ref="A1:C12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField axis="axisCol" compact="0" showAll="0" defaultSubtotal="0" outline="0">
+      <items count="2">
+        <item x="0"/>
+        <item x="1"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0" outline="0">
+      <items count="10">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" showAll="0"/>
+    <pivotField compact="0" showAll="0"/>
+    <pivotField compact="0" showAll="0"/>
+    <pivotField compact="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" showAll="0" outline="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <dataFields count="1">
+    <dataField name="Sum - Percentage Relative Importance" fld="6" subtotal="sum" numFmtId="164"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1849,51 +1526,51 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>0.000232995435173744</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>0.000228728567364445</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>0.000230893800397467</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>0.000230887440571793</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>28.4042171216637</v>
       </c>
     </row>
@@ -1901,22 +1578,22 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>0.00014501681563539</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>0.000140218767829881</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>0.000142630624491342</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>0.000142628057939601</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>17.5463780763681</v>
       </c>
     </row>
@@ -1924,22 +1601,22 @@
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>0.000137609572220199</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>0.000135240967717887</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>0.000136491133712001</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>0.000136477960963409</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>16.7897813147668</v>
       </c>
     </row>
@@ -1947,22 +1624,22 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>0.000102557749521282</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>0.00010483069440359</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>0.000103760481892498</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>0.000103747229906486</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>12.7631838125845</v>
       </c>
     </row>
@@ -1970,22 +1647,22 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>9.55230633552517E-005</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>9.32524626982012E-005</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>9.4402724089783E-005</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>9.43997318771717E-005</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>11.6132366222505</v>
       </c>
     </row>
@@ -1993,22 +1670,22 @@
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>5.53198529773535E-005</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>5.26345179471255E-005</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>5.39934536762319E-005</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>5.39902000334334E-005</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>6.64197827475527</v>
       </c>
     </row>
@@ -2016,22 +1693,22 @@
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>2.21284191331828E-005</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>2.19126829460459E-005</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>2.20446143106668E-005</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <v>2.20398016564563E-005</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>2.7113788000683</v>
       </c>
     </row>
@@ -2039,22 +1716,22 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>1.18239719762991E-005</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>1.17709327395188E-005</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>1.18174919522494E-005</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <v>1.18134840333813E-005</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>1.4533175326318</v>
       </c>
     </row>
@@ -2062,22 +1739,22 @@
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>9.93716412378554E-006</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>1.14602157303967E-005</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>1.07206486686124E-005</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>1.07162569203082E-005</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>1.31833454233002</v>
       </c>
     </row>
@@ -2085,22 +1762,22 @@
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>6.33582934583821E-006</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>5.95974193140503E-006</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>6.16690302554721E-006</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="1" t="n">
         <v>6.1630795481621E-006</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <v>0.758193902581064</v>
       </c>
     </row>
@@ -2126,265 +1803,265 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>0.000545380454899047</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>0.000551867620766755</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>0.000548673256131186</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>0.000548663412471529</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>29.2528246248874</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>0.000499030163925163</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>0.000484718056299571</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>0.000491946849271153</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>0.000491932301439395</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>26.2281191240734</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>0.000371525425160168</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>0.000351799699663147</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>0.00036169720707843</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>0.000361690278145076</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>19.2840674894714</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>0.000223139309298626</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>0.000225803621144438</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>0.000224488728146164</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>0.000224485275561237</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>11.9687740199064</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>0.000105759357481583</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>0.000116389925737259</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>0.000111061958071466</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>0.000111064494779057</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>5.92157252328551</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>6.65225985324591E-005</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>7.23716351652692E-005</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>6.95061471338585E-005</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>6.94943410768596E-005</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>3.70519652984693</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>5.07475121328538E-005</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>4.95563624320905E-005</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>5.01389194685773E-005</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <v>5.01415230313563E-005</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>2.67337159052342</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>1.83021132890149E-005</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>1.68566993200558E-005</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>1.76426693062476E-005</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <v>1.76300167059051E-005</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>0.939971164668175</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>6.79583742058121E-007</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>1.73841082973247E-007</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>4.28283769386144E-007</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>4.27969498012052E-007</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>0.0228178449402206</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>1.17858073633847E-007</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>1.52610812875764E-009</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>6.20955145210286E-008</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="1" t="n">
         <v>6.16148297930834E-008</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <v>0.00328508839711066</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2397,60 +2074,60 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>0.000232995435173744</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>0.000228728567364445</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>0.000230893800397467</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>0.000230887440571793</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>28.4042171216637</v>
       </c>
     </row>
@@ -2458,22 +2135,22 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>0.00014501681563539</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>0.000140218767829881</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>0.000142630624491342</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>0.000142628057939601</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>17.5463780763681</v>
       </c>
     </row>
@@ -2481,22 +2158,22 @@
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>0.000137609572220199</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>0.000135240967717887</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>0.000136491133712001</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>0.000136477960963409</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>16.7897813147668</v>
       </c>
     </row>
@@ -2504,22 +2181,22 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>0.000102557749521282</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>0.00010483069440359</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>0.000103760481892498</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>0.000103747229906486</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>12.7631838125845</v>
       </c>
     </row>
@@ -2527,22 +2204,22 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>9.55230633552517E-005</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>9.32524626982012E-005</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>9.4402724089783E-005</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>9.43997318771717E-005</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>11.6132366222505</v>
       </c>
     </row>
@@ -2550,22 +2227,22 @@
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>5.53198529773535E-005</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>5.26345179471255E-005</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>5.39934536762319E-005</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>5.39902000334334E-005</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>6.64197827475527</v>
       </c>
     </row>
@@ -2573,22 +2250,22 @@
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>2.21284191331828E-005</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>2.19126829460459E-005</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>2.20446143106668E-005</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <v>2.20398016564563E-005</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>2.7113788000683</v>
       </c>
     </row>
@@ -2596,22 +2273,22 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>1.18239719762991E-005</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>1.17709327395188E-005</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>1.18174919522494E-005</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <v>1.18134840333813E-005</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>1.4533175326318</v>
       </c>
     </row>
@@ -2619,22 +2296,22 @@
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>9.93716412378554E-006</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>1.14602157303967E-005</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>1.07206486686124E-005</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>1.07162569203082E-005</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>1.31833454233002</v>
       </c>
     </row>
@@ -2642,259 +2319,265 @@
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>6.33582934583821E-006</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>5.95974193140503E-006</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>6.16690302554721E-006</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="1" t="n">
         <v>6.1630795481621E-006</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <v>0.758193902581064</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>0.000545380454899047</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>0.000551867620766755</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>0.000548673256131186</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="1" t="n">
         <v>0.000548663412471529</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="1" t="n">
         <v>29.2528246248874</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>0.000499030163925163</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>0.000484718056299571</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>0.000491946849271153</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="1" t="n">
         <v>0.000491932301439395</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="1" t="n">
         <v>26.2281191240734</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>0.000371525425160168</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>0.000351799699663147</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>0.00036169720707843</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="1" t="n">
         <v>0.000361690278145076</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="1" t="n">
         <v>19.2840674894714</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>0.000223139309298626</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>0.000225803621144438</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>0.000224488728146164</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="1" t="n">
         <v>0.000224485275561237</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="1" t="n">
         <v>11.9687740199064</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>0.000105759357481583</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>0.000116389925737259</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>0.000111061958071466</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="1" t="n">
         <v>0.000111064494779057</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="1" t="n">
         <v>5.92157252328551</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>6.65225985324591E-005</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>7.23716351652692E-005</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>6.95061471338585E-005</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="1" t="n">
         <v>6.94943410768596E-005</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="1" t="n">
         <v>3.70519652984693</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="1" t="n">
         <v>5.07475121328538E-005</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>4.95563624320905E-005</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>5.01389194685773E-005</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="1" t="n">
         <v>5.01415230313563E-005</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="1" t="n">
         <v>2.67337159052342</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="1" t="n">
         <v>1.83021132890149E-005</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <v>1.68566993200558E-005</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>1.76426693062476E-005</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="1" t="n">
         <v>1.76300167059051E-005</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="G19" s="1" t="n">
         <v>0.939971164668175</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="1" t="n">
         <v>6.79583742058121E-007</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="1" t="n">
         <v>1.73841082973247E-007</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>4.28283769386144E-007</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="1" t="n">
         <v>4.27969498012052E-007</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="G20" s="1" t="n">
         <v>0.0228178449402206</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21" s="1" t="n">
         <v>1.17858073633847E-007</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="1" t="n">
         <v>1.52610812875764E-009</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="1" t="n">
         <v>6.20955145210286E-008</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="1" t="n">
         <v>6.16148297930834E-008</v>
       </c>
-      <c r="G21" s="0" t="n">
+      <c r="G21" s="1" t="n">
         <v>0.00328508839711066</v>
       </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2907,10 +2590,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X24" activeCellId="0" sqref="X24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2923,128 +2606,330 @@
         <v>23</v>
       </c>
       <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="B3" s="9" t="n">
+        <v>0.00328508839711066</v>
+      </c>
+      <c r="C3" s="10" t="n">
+        <v>12.7631838125845</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="B4" s="12" t="n">
+        <v>5.92157252328551</v>
+      </c>
+      <c r="C4" s="13" t="n">
+        <v>6.64197827475527</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="B5" s="12" t="n">
+        <v>0.0228178449402206</v>
+      </c>
+      <c r="C5" s="13" t="n">
+        <v>17.5463780763681</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="B6" s="12" t="n">
+        <v>11.9687740199064</v>
+      </c>
+      <c r="C6" s="13" t="n">
+        <v>1.4533175326318</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="B7" s="12" t="n">
+        <v>29.2528246248874</v>
+      </c>
+      <c r="C7" s="13" t="n">
+        <v>1.31833454233002</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="B8" s="12" t="n">
+        <v>3.70519652984693</v>
+      </c>
+      <c r="C8" s="13" t="n">
+        <v>0.758193902581064</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="B9" s="12" t="n">
+        <v>26.2281191240734</v>
+      </c>
+      <c r="C9" s="13" t="n">
+        <v>28.4042171216637</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="B10" s="12" t="n">
+        <v>19.2840674894714</v>
+      </c>
+      <c r="C10" s="13" t="n">
+        <v>16.7897813147668</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="B11" s="12" t="n">
+        <v>2.67337159052342</v>
+      </c>
+      <c r="C11" s="13" t="n">
+        <v>11.6132366222505</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="11" t="n">
-        <v>0.00328508839711066</v>
-      </c>
-      <c r="C3" s="12" t="n">
-        <v>5.92157252328551</v>
-      </c>
-      <c r="D3" s="12" t="n">
-        <v>0.0228178449402206</v>
-      </c>
-      <c r="E3" s="12" t="n">
-        <v>11.9687740199064</v>
-      </c>
-      <c r="F3" s="12" t="n">
-        <v>29.2528246248874</v>
-      </c>
-      <c r="G3" s="12" t="n">
-        <v>3.70519652984693</v>
-      </c>
-      <c r="H3" s="12" t="n">
-        <v>26.2281191240734</v>
-      </c>
-      <c r="I3" s="12" t="n">
-        <v>19.2840674894714</v>
-      </c>
-      <c r="J3" s="12" t="n">
-        <v>2.67337159052342</v>
-      </c>
-      <c r="K3" s="13" t="n">
+      <c r="B12" s="15" t="n">
         <v>0.939971164668175</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="15" t="n">
-        <v>12.7631838125845</v>
-      </c>
-      <c r="C4" s="16" t="n">
-        <v>6.64197827475527</v>
-      </c>
-      <c r="D4" s="16" t="n">
-        <v>17.5463780763681</v>
-      </c>
-      <c r="E4" s="16" t="n">
-        <v>1.4533175326318</v>
-      </c>
-      <c r="F4" s="16" t="n">
-        <v>1.31833454233002</v>
-      </c>
-      <c r="G4" s="16" t="n">
-        <v>0.758193902581064</v>
-      </c>
-      <c r="H4" s="16" t="n">
-        <v>28.4042171216637</v>
-      </c>
-      <c r="I4" s="16" t="n">
-        <v>16.7897813147668</v>
-      </c>
-      <c r="J4" s="16" t="n">
-        <v>11.6132366222505</v>
-      </c>
-      <c r="K4" s="17" t="n">
+      <c r="C12" s="16" t="n">
         <v>2.7113788000683</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P28" activeCellId="0" sqref="P28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="4"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="20" t="n">
+        <v>0.00328508839711066</v>
+      </c>
+      <c r="C3" s="21" t="n">
+        <v>5.92157252328551</v>
+      </c>
+      <c r="D3" s="21" t="n">
+        <v>0.0228178449402206</v>
+      </c>
+      <c r="E3" s="21" t="n">
+        <v>11.9687740199064</v>
+      </c>
+      <c r="F3" s="21" t="n">
+        <v>29.2528246248874</v>
+      </c>
+      <c r="G3" s="21" t="n">
+        <v>3.70519652984693</v>
+      </c>
+      <c r="H3" s="21" t="n">
+        <v>26.2281191240734</v>
+      </c>
+      <c r="I3" s="21" t="n">
+        <v>19.2840674894714</v>
+      </c>
+      <c r="J3" s="21" t="n">
+        <v>2.67337159052342</v>
+      </c>
+      <c r="K3" s="22" t="n">
+        <v>0.939971164668175</v>
+      </c>
+      <c r="L3" s="23" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="24" t="n">
+        <v>12.7631838125845</v>
+      </c>
+      <c r="C4" s="25" t="n">
+        <v>6.64197827475527</v>
+      </c>
+      <c r="D4" s="25" t="n">
+        <v>17.5463780763681</v>
+      </c>
+      <c r="E4" s="25" t="n">
+        <v>1.4533175326318</v>
+      </c>
+      <c r="F4" s="25" t="n">
+        <v>1.31833454233002</v>
+      </c>
+      <c r="G4" s="25" t="n">
+        <v>0.758193902581064</v>
+      </c>
+      <c r="H4" s="25" t="n">
+        <v>28.4042171216637</v>
+      </c>
+      <c r="I4" s="25" t="n">
+        <v>16.7897813147668</v>
+      </c>
+      <c r="J4" s="25" t="n">
+        <v>11.6132366222505</v>
+      </c>
+      <c r="K4" s="26" t="n">
+        <v>2.7113788000683</v>
+      </c>
+      <c r="L4" s="27" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="29" t="n">
+        <v>12.7664689009816</v>
+      </c>
+      <c r="C5" s="30" t="n">
+        <v>12.5635507980408</v>
+      </c>
+      <c r="D5" s="30" t="n">
+        <v>17.5691959213083</v>
+      </c>
+      <c r="E5" s="30" t="n">
+        <v>13.4220915525382</v>
+      </c>
+      <c r="F5" s="30" t="n">
+        <v>30.5711591672174</v>
+      </c>
+      <c r="G5" s="30" t="n">
+        <v>4.46339043242799</v>
+      </c>
+      <c r="H5" s="30" t="n">
+        <v>54.6323362457371</v>
+      </c>
+      <c r="I5" s="30" t="n">
+        <v>36.0738488042382</v>
+      </c>
+      <c r="J5" s="30" t="n">
+        <v>14.2866082127739</v>
+      </c>
+      <c r="K5" s="31" t="n">
+        <v>3.65134996473647</v>
+      </c>
+      <c r="L5" s="32" t="n">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>